<commit_message>
DB views now created on-demand in app. Improved app translation for spanish and added polish to the app.
</commit_message>
<xml_diff>
--- a/assets/i18n_data/app_text.xlsx
+++ b/assets/i18n_data/app_text.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="639">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="640">
   <si>
     <t>key</t>
   </si>
@@ -1218,13 +1218,16 @@
     <t>Deciembre</t>
   </si>
   <si>
+    <t>Verificar el filtrado de la pantalla de tus alimentos.</t>
+  </si>
+  <si>
+    <t>Agreguar a favoritos tocando la estrella de la comida ☆.</t>
+  </si>
+  <si>
+    <t>¡No hay favoritos disponibles!</t>
+  </si>
+  <si>
     <t>¡No hay alimentos disponibles!</t>
-  </si>
-  <si>
-    <t>Agreguar a favoritos tocando la estrella de la comida ☆.</t>
-  </si>
-  <si>
-    <t>¡No hay favoritos disponibles!</t>
   </si>
   <si>
     <t>¡No se encontraron alimentos!</t>
@@ -1955,19 +1958,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1986,24 +1982,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2023,15 +2004,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2045,7 +2019,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2061,30 +2058,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2114,7 +2102,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2126,6 +2122,30 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2141,7 +2161,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2153,43 +2203,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2207,13 +2227,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2225,73 +2287,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2303,13 +2299,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2323,17 +2319,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2356,8 +2355,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2379,20 +2378,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2411,166 +2416,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4015,7 +4011,7 @@
   <dimension ref="B1:D98"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -5112,8 +5108,8 @@
   <sheetPr/>
   <dimension ref="B1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -5393,7 +5389,7 @@
       <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>397</v>
       </c>
     </row>
@@ -5427,7 +5423,7 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -5438,7 +5434,7 @@
         <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -5449,7 +5445,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -5460,7 +5456,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -5471,7 +5467,7 @@
         <v>93</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -5482,7 +5478,7 @@
         <v>96</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -5493,7 +5489,7 @@
         <v>99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -5504,7 +5500,7 @@
         <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -5515,7 +5511,7 @@
         <v>105</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -5526,7 +5522,7 @@
         <v>108</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -5537,7 +5533,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -5548,7 +5544,7 @@
         <v>114</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -5559,7 +5555,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -5581,7 +5577,7 @@
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -5603,7 +5599,7 @@
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -5614,7 +5610,7 @@
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -5625,7 +5621,7 @@
         <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -5636,7 +5632,7 @@
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -5647,7 +5643,7 @@
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -5669,7 +5665,7 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -5680,7 +5676,7 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -5691,7 +5687,7 @@
         <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -5702,7 +5698,7 @@
         <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -5724,7 +5720,7 @@
         <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -5746,7 +5742,7 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -5757,7 +5753,7 @@
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -5768,7 +5764,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -5779,7 +5775,7 @@
         <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -5790,7 +5786,7 @@
         <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -5801,7 +5797,7 @@
         <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -5812,7 +5808,7 @@
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -5823,7 +5819,7 @@
         <v>187</v>
       </c>
       <c r="D64" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -5845,7 +5841,7 @@
         <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -5856,7 +5852,7 @@
         <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -5867,7 +5863,7 @@
         <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -5878,7 +5874,7 @@
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -5889,7 +5885,7 @@
         <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -5900,7 +5896,7 @@
         <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -5911,7 +5907,7 @@
         <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -5922,7 +5918,7 @@
         <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -5933,7 +5929,7 @@
         <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -5944,7 +5940,7 @@
         <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -5955,7 +5951,7 @@
         <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -5966,7 +5962,7 @@
         <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -5977,7 +5973,7 @@
         <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -5988,7 +5984,7 @@
         <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -5999,7 +5995,7 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -6010,7 +6006,7 @@
         <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -6021,7 +6017,7 @@
         <v>240</v>
       </c>
       <c r="D82" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -6032,7 +6028,7 @@
         <v>243</v>
       </c>
       <c r="D83" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -6043,7 +6039,7 @@
         <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -6054,7 +6050,7 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -6065,7 +6061,7 @@
         <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -6076,7 +6072,7 @@
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -6087,7 +6083,7 @@
         <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -6098,7 +6094,7 @@
         <v>261</v>
       </c>
       <c r="D89" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -6109,7 +6105,7 @@
         <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -6120,7 +6116,7 @@
         <v>267</v>
       </c>
       <c r="D91" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -6131,7 +6127,7 @@
         <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -6142,7 +6138,7 @@
         <v>273</v>
       </c>
       <c r="D93" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -6153,7 +6149,7 @@
         <v>276</v>
       </c>
       <c r="D94" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -6164,7 +6160,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -6175,7 +6171,7 @@
         <v>282</v>
       </c>
       <c r="D96" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -6186,7 +6182,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -6229,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -6240,7 +6236,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -6251,7 +6247,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -6262,7 +6258,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -6273,7 +6269,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -6284,7 +6280,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -6295,7 +6291,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -6306,7 +6302,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -6317,7 +6313,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -6328,7 +6324,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -6339,7 +6335,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -6350,7 +6346,7 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -6361,7 +6357,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -6372,7 +6368,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -6383,7 +6379,7 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -6394,7 +6390,7 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -6405,7 +6401,7 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -6416,7 +6412,7 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -6427,7 +6423,7 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -6438,7 +6434,7 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -6449,7 +6445,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -6460,7 +6456,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -6471,7 +6467,7 @@
         <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -6482,7 +6478,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -6493,7 +6489,7 @@
         <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -6504,7 +6500,7 @@
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -6515,7 +6511,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -6526,7 +6522,7 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -6537,7 +6533,7 @@
         <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -6548,7 +6544,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -6559,7 +6555,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -6570,7 +6566,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -6581,7 +6577,7 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -6592,7 +6588,7 @@
         <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -6603,7 +6599,7 @@
         <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -6614,7 +6610,7 @@
         <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -6625,7 +6621,7 @@
         <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -6636,7 +6632,7 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -6647,7 +6643,7 @@
         <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -6658,7 +6654,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -6669,7 +6665,7 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -6680,7 +6676,7 @@
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -6691,7 +6687,7 @@
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -6702,7 +6698,7 @@
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -6713,7 +6709,7 @@
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -6724,7 +6720,7 @@
         <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -6735,7 +6731,7 @@
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -6746,7 +6742,7 @@
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -6757,7 +6753,7 @@
         <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -6768,7 +6764,7 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -6779,7 +6775,7 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -6790,7 +6786,7 @@
         <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -6801,7 +6797,7 @@
         <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -6812,7 +6808,7 @@
         <v>159</v>
       </c>
       <c r="D54" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -6845,7 +6841,7 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -6867,7 +6863,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -6878,7 +6874,7 @@
         <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -6889,7 +6885,7 @@
         <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -6900,7 +6896,7 @@
         <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -6911,7 +6907,7 @@
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -6922,7 +6918,7 @@
         <v>187</v>
       </c>
       <c r="D64" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -6933,7 +6929,7 @@
         <v>190</v>
       </c>
       <c r="D65" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -6944,7 +6940,7 @@
         <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -6955,7 +6951,7 @@
         <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -6977,7 +6973,7 @@
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -6988,7 +6984,7 @@
         <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -6999,7 +6995,7 @@
         <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -7010,7 +7006,7 @@
         <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -7021,7 +7017,7 @@
         <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -7032,7 +7028,7 @@
         <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -7043,7 +7039,7 @@
         <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -7054,7 +7050,7 @@
         <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -7065,7 +7061,7 @@
         <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -7076,7 +7072,7 @@
         <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -7087,7 +7083,7 @@
         <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -7098,7 +7094,7 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -7109,7 +7105,7 @@
         <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -7120,7 +7116,7 @@
         <v>240</v>
       </c>
       <c r="D82" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -7131,7 +7127,7 @@
         <v>243</v>
       </c>
       <c r="D83" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -7142,7 +7138,7 @@
         <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -7153,7 +7149,7 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -7164,7 +7160,7 @@
         <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -7175,7 +7171,7 @@
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -7186,7 +7182,7 @@
         <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -7208,7 +7204,7 @@
         <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -7219,7 +7215,7 @@
         <v>267</v>
       </c>
       <c r="D91" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -7230,7 +7226,7 @@
         <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -7241,7 +7237,7 @@
         <v>273</v>
       </c>
       <c r="D93" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -7252,7 +7248,7 @@
         <v>276</v>
       </c>
       <c r="D94" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -7263,7 +7259,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -7274,7 +7270,7 @@
         <v>282</v>
       </c>
       <c r="D96" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -7285,7 +7281,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -7328,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -7339,7 +7335,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -7350,7 +7346,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -7361,7 +7357,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -7372,7 +7368,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -7383,7 +7379,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -7394,7 +7390,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -7405,7 +7401,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -7416,7 +7412,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -7427,7 +7423,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -7438,7 +7434,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -7449,7 +7445,7 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -7460,7 +7456,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -7471,7 +7467,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -7482,7 +7478,7 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -7493,7 +7489,7 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -7504,7 +7500,7 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -7515,7 +7511,7 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -7526,7 +7522,7 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -7537,7 +7533,7 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -7548,7 +7544,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -7559,7 +7555,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -7570,7 +7566,7 @@
         <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -7581,7 +7577,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -7592,7 +7588,7 @@
         <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -7603,7 +7599,7 @@
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -7614,7 +7610,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -7625,7 +7621,7 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -7636,7 +7632,7 @@
         <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -7647,7 +7643,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -7658,7 +7654,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -7669,7 +7665,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -7680,7 +7676,7 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -7691,7 +7687,7 @@
         <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -7702,7 +7698,7 @@
         <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -7713,7 +7709,7 @@
         <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -7724,7 +7720,7 @@
         <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -7735,7 +7731,7 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -7746,7 +7742,7 @@
         <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -7757,7 +7753,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -7768,7 +7764,7 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -7779,7 +7775,7 @@
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -7790,7 +7786,7 @@
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -7801,7 +7797,7 @@
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -7812,7 +7808,7 @@
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -7823,7 +7819,7 @@
         <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -7834,7 +7830,7 @@
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -7845,7 +7841,7 @@
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -7856,7 +7852,7 @@
         <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -7867,7 +7863,7 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -7878,7 +7874,7 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -7889,7 +7885,7 @@
         <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -7911,7 +7907,7 @@
         <v>159</v>
       </c>
       <c r="D54" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -7922,7 +7918,7 @@
         <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -7944,7 +7940,7 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -7955,7 +7951,7 @@
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -7966,7 +7962,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -7977,7 +7973,7 @@
         <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -7988,7 +7984,7 @@
         <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -7999,7 +7995,7 @@
         <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -8010,7 +8006,7 @@
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -8021,7 +8017,7 @@
         <v>187</v>
       </c>
       <c r="D64" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -8032,7 +8028,7 @@
         <v>190</v>
       </c>
       <c r="D65" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -8043,7 +8039,7 @@
         <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -8054,7 +8050,7 @@
         <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -8065,7 +8061,7 @@
         <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -8076,7 +8072,7 @@
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -8087,7 +8083,7 @@
         <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -8098,7 +8094,7 @@
         <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -8109,7 +8105,7 @@
         <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -8120,7 +8116,7 @@
         <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -8131,7 +8127,7 @@
         <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -8142,7 +8138,7 @@
         <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -8153,7 +8149,7 @@
         <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -8164,7 +8160,7 @@
         <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -8175,7 +8171,7 @@
         <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -8186,7 +8182,7 @@
         <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -8197,7 +8193,7 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -8208,7 +8204,7 @@
         <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -8219,7 +8215,7 @@
         <v>240</v>
       </c>
       <c r="D82" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -8241,7 +8237,7 @@
         <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -8252,7 +8248,7 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -8263,7 +8259,7 @@
         <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -8274,7 +8270,7 @@
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -8285,7 +8281,7 @@
         <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -8296,7 +8292,7 @@
         <v>261</v>
       </c>
       <c r="D89" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -8307,7 +8303,7 @@
         <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -8318,7 +8314,7 @@
         <v>267</v>
       </c>
       <c r="D91" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -8329,7 +8325,7 @@
         <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -8340,7 +8336,7 @@
         <v>273</v>
       </c>
       <c r="D93" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -8351,7 +8347,7 @@
         <v>276</v>
       </c>
       <c r="D94" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -8362,7 +8358,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -8373,7 +8369,7 @@
         <v>282</v>
       </c>
       <c r="D96" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -8384,7 +8380,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="98" spans="2:4">

</xml_diff>

<commit_message>
small fixes to spanish app text, build code bump
</commit_message>
<xml_diff>
--- a/assets/i18n_data/app_text.xlsx
+++ b/assets/i18n_data/app_text.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="640">
   <si>
     <t>key</t>
   </si>
@@ -1176,99 +1176,99 @@
     <t>Hoy en día, casi todos los alimentos están disponibles durante todo el año, generando que la gente pierda la conciencia sobre la temporada de estos. Sin embargo, comprar alimentos locales y en temporada a menudo tiene ventajas sorprendentes:</t>
   </si>
   <si>
+    <t>Sobre la aplicación</t>
+  </si>
+  <si>
+    <t>Esta aplicación te permite comer más barato y sabroso! a la vez, aumentar la conciencia sobre el origen de nuestra comida.</t>
+  </si>
+  <si>
+    <t>Calendario de alimentos de temporada</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Augusto</t>
+  </si>
+  <si>
+    <t>Volver</t>
+  </si>
+  <si>
+    <t>Europa Central</t>
+  </si>
+  <si>
+    <t>El código fuente de la aplicación está disponible en GitHub:</t>
+  </si>
+  <si>
+    <t>Hacia GitHub repo</t>
+  </si>
+  <si>
+    <t>¡Enséñame el código!</t>
+  </si>
+  <si>
+    <t>Si ha encontrado un error o margen de mejora, no dude en contactarme a través de mi página web.</t>
+  </si>
+  <si>
+    <t>A la pagina web</t>
+  </si>
+  <si>
+    <t>¿Algo falta o está mal?</t>
+  </si>
+  <si>
+    <t>Contribuir</t>
+  </si>
+  <si>
+    <t>Deciembre</t>
+  </si>
+  <si>
+    <t>Verificar el filtrado de la pantalla de tus alimentos.</t>
+  </si>
+  <si>
+    <t>Agreguar a favoritos tocando la estrella de la comida ☆.</t>
+  </si>
+  <si>
+    <t>¡No hay favoritos disponibles!</t>
+  </si>
+  <si>
+    <t>¡No hay alimentos disponibles!</t>
+  </si>
+  <si>
+    <t>¡No se encontraron alimentos!</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Importado de lejos, principalmente por avión.</t>
+  </si>
+  <si>
+    <t>Importado no muy lejos, principalmente por transporte terrestre.</t>
+  </si>
+  <si>
+    <t>En temporada o regionalmente disponible</t>
+  </si>
+  <si>
+    <t>Importados de lejos, en su mayoría por transporte marítimo.</t>
+  </si>
+  <si>
+    <t>El color del nombre indica su clasificación. Desde verde (bueno) a rojo (malo).</t>
+  </si>
+  <si>
+    <t>Esta aplicación le muestra de un vistazo qué alimentos están en temporada en este momento</t>
+  </si>
+  <si>
+    <t>¿Cómo utilizar la aplicación?</t>
+  </si>
+  <si>
+    <t>Al tocar la estrella de un alimento ☆, la puedes agregar o eliminar de tu lista de favoritos. Tocar la estrella de la barra de menú te permite restringir la vista a sus favoritos.</t>
+  </si>
+  <si>
+    <t>Un ícono negro indica disponibilidad abundante, un ícono gris indica disponibilidad limitada de esa categoría específica.</t>
+  </si>
+  <si>
     <t>Explicación</t>
   </si>
   <si>
-    <t>Esta aplicación te permite comer más barato y sabroso! a la vez, aumentar la conciencia sobre el origen de nuestra comida.</t>
-  </si>
-  <si>
-    <t>Calendario de alimentos de temporada</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Augusto</t>
-  </si>
-  <si>
-    <t>Volver</t>
-  </si>
-  <si>
-    <t>Europa Central</t>
-  </si>
-  <si>
-    <t>El código fuente de la aplicación está disponible en GitHub:</t>
-  </si>
-  <si>
-    <t>Hacia GitHub repo</t>
-  </si>
-  <si>
-    <t>¡Enséñame el código!</t>
-  </si>
-  <si>
-    <t>Si ha encontrado un error o margen de mejora, no dude en contactarme a través de mi página web.</t>
-  </si>
-  <si>
-    <t>A la pagina web</t>
-  </si>
-  <si>
-    <t>¿Algo falta o está mal?</t>
-  </si>
-  <si>
-    <t>Contribuir</t>
-  </si>
-  <si>
-    <t>Deciembre</t>
-  </si>
-  <si>
-    <t>Verificar el filtrado de la pantalla de tus alimentos.</t>
-  </si>
-  <si>
-    <t>Agreguar a favoritos tocando la estrella de la comida ☆.</t>
-  </si>
-  <si>
-    <t>¡No hay favoritos disponibles!</t>
-  </si>
-  <si>
-    <t>¡No hay alimentos disponibles!</t>
-  </si>
-  <si>
-    <t>¡No se encontraron alimentos!</t>
-  </si>
-  <si>
-    <t>Sobre la aplicación</t>
-  </si>
-  <si>
-    <t>Febrero</t>
-  </si>
-  <si>
-    <t>Importado de lejos, principalmente por avión.</t>
-  </si>
-  <si>
-    <t>Importado no muy lejos, principalmente por transporte terrestre.</t>
-  </si>
-  <si>
-    <t>En temporada o regionalmente disponible</t>
-  </si>
-  <si>
-    <t>Importados de lejos, en su mayoría por transporte marítimo.</t>
-  </si>
-  <si>
-    <t>El color del nombre indica su clasificación. Desde verde (bueno) a rojo (malo).</t>
-  </si>
-  <si>
-    <t>Esta aplicación le muestra de un vistazo qué alimentos están en temporada en este momento</t>
-  </si>
-  <si>
-    <t>¿Cómo utilizar la aplicación?</t>
-  </si>
-  <si>
-    <t>Al tocar la estrella de un alimento ☆, la puedes agregar o eliminar de tu lista de favoritos. Tocar la estrella de la barra de menú te permite restringir la vista a sus favoritos.</t>
-  </si>
-  <si>
-    <t>Un ícono negro indica disponibilidad abundante, un ícono gris indica disponibilidad limitada de esa categoría específica.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Licencia: </t>
   </si>
   <si>
@@ -1411,9 +1411,6 @@
   </si>
   <si>
     <t>Soporte</t>
-  </si>
-  <si>
-    <t>Ir a la pagina web</t>
   </si>
   <si>
     <t>fr</t>
@@ -1990,6 +1987,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -1998,8 +2002,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2009,6 +2014,30 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2028,19 +2057,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2052,16 +2079,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2075,45 +2110,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2134,49 +2131,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2194,13 +2161,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2212,7 +2191,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2224,55 +2293,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2284,31 +2305,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2333,9 +2330,35 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2355,26 +2378,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2396,168 +2410,151 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5111,8 +5108,8 @@
   <sheetPr/>
   <dimension ref="B1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
@@ -5448,7 +5445,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>403</v>
+        <v>383</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -5459,7 +5456,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -5470,7 +5467,7 @@
         <v>93</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -5481,7 +5478,7 @@
         <v>96</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -5492,7 +5489,7 @@
         <v>99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -5503,7 +5500,7 @@
         <v>102</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -5514,7 +5511,7 @@
         <v>105</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -5525,7 +5522,7 @@
         <v>108</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -5536,7 +5533,7 @@
         <v>111</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -5547,7 +5544,7 @@
         <v>114</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -5558,7 +5555,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -5569,7 +5566,7 @@
         <v>120</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>383</v>
+        <v>413</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -6185,7 +6182,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>462</v>
+        <v>394</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -6228,7 +6225,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -6239,7 +6236,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -6250,7 +6247,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -6261,7 +6258,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -6272,7 +6269,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -6283,7 +6280,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -6294,7 +6291,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -6305,7 +6302,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -6316,7 +6313,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -6327,7 +6324,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -6338,7 +6335,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -6349,7 +6346,7 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -6360,7 +6357,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -6371,7 +6368,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -6382,7 +6379,7 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -6393,7 +6390,7 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -6404,7 +6401,7 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -6415,7 +6412,7 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -6426,7 +6423,7 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -6437,7 +6434,7 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -6448,7 +6445,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -6459,7 +6456,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -6470,7 +6467,7 @@
         <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -6481,7 +6478,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -6492,7 +6489,7 @@
         <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -6503,7 +6500,7 @@
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -6514,7 +6511,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -6525,7 +6522,7 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -6536,7 +6533,7 @@
         <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -6547,7 +6544,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -6558,7 +6555,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -6569,7 +6566,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -6580,7 +6577,7 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -6591,7 +6588,7 @@
         <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -6602,7 +6599,7 @@
         <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -6613,7 +6610,7 @@
         <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -6624,7 +6621,7 @@
         <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -6635,7 +6632,7 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -6646,7 +6643,7 @@
         <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -6657,7 +6654,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -6668,7 +6665,7 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -6679,7 +6676,7 @@
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -6690,7 +6687,7 @@
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -6701,7 +6698,7 @@
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -6712,7 +6709,7 @@
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -6723,7 +6720,7 @@
         <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -6734,7 +6731,7 @@
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -6745,7 +6742,7 @@
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -6756,7 +6753,7 @@
         <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -6767,7 +6764,7 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -6778,7 +6775,7 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -6789,7 +6786,7 @@
         <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -6800,7 +6797,7 @@
         <v>156</v>
       </c>
       <c r="D53" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="54" spans="2:4">
@@ -6811,7 +6808,7 @@
         <v>159</v>
       </c>
       <c r="D54" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -6844,7 +6841,7 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -6866,7 +6863,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -6877,7 +6874,7 @@
         <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -6888,7 +6885,7 @@
         <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -6899,7 +6896,7 @@
         <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -6910,7 +6907,7 @@
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -6921,7 +6918,7 @@
         <v>187</v>
       </c>
       <c r="D64" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -6932,7 +6929,7 @@
         <v>190</v>
       </c>
       <c r="D65" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -6943,7 +6940,7 @@
         <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -6954,7 +6951,7 @@
         <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -6976,7 +6973,7 @@
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -6987,7 +6984,7 @@
         <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -6998,7 +6995,7 @@
         <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -7009,7 +7006,7 @@
         <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -7020,7 +7017,7 @@
         <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -7031,7 +7028,7 @@
         <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -7042,7 +7039,7 @@
         <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -7053,7 +7050,7 @@
         <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -7064,7 +7061,7 @@
         <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -7075,7 +7072,7 @@
         <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -7086,7 +7083,7 @@
         <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -7097,7 +7094,7 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -7108,7 +7105,7 @@
         <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -7119,7 +7116,7 @@
         <v>240</v>
       </c>
       <c r="D82" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -7130,7 +7127,7 @@
         <v>243</v>
       </c>
       <c r="D83" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="84" spans="2:4">
@@ -7141,7 +7138,7 @@
         <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -7152,7 +7149,7 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -7163,7 +7160,7 @@
         <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -7174,7 +7171,7 @@
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -7185,7 +7182,7 @@
         <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -7207,7 +7204,7 @@
         <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -7218,7 +7215,7 @@
         <v>267</v>
       </c>
       <c r="D91" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -7229,7 +7226,7 @@
         <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -7240,7 +7237,7 @@
         <v>273</v>
       </c>
       <c r="D93" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -7251,7 +7248,7 @@
         <v>276</v>
       </c>
       <c r="D94" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -7262,7 +7259,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -7273,7 +7270,7 @@
         <v>282</v>
       </c>
       <c r="D96" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -7284,7 +7281,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="98" spans="2:4">
@@ -7327,7 +7324,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="2" spans="2:4">
@@ -7338,7 +7335,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="3" spans="2:4">
@@ -7349,7 +7346,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="2:4">
@@ -7360,7 +7357,7 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -7371,7 +7368,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -7382,7 +7379,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -7393,7 +7390,7 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="2:4">
@@ -7404,7 +7401,7 @@
         <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -7415,7 +7412,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -7426,7 +7423,7 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -7437,7 +7434,7 @@
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -7448,7 +7445,7 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -7459,7 +7456,7 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -7470,7 +7467,7 @@
         <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -7481,7 +7478,7 @@
         <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -7492,7 +7489,7 @@
         <v>46</v>
       </c>
       <c r="D16" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="17" spans="2:4">
@@ -7503,7 +7500,7 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="18" spans="2:4">
@@ -7514,7 +7511,7 @@
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="19" spans="2:4">
@@ -7525,7 +7522,7 @@
         <v>55</v>
       </c>
       <c r="D19" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -7536,7 +7533,7 @@
         <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="21" spans="2:4">
@@ -7547,7 +7544,7 @@
         <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" spans="2:4">
@@ -7558,7 +7555,7 @@
         <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="23" spans="2:4">
@@ -7569,7 +7566,7 @@
         <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="24" spans="2:4">
@@ -7580,7 +7577,7 @@
         <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="25" spans="2:4">
@@ -7591,7 +7588,7 @@
         <v>73</v>
       </c>
       <c r="D25" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="26" spans="2:4">
@@ -7602,7 +7599,7 @@
         <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="27" spans="2:4">
@@ -7613,7 +7610,7 @@
         <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="28" spans="2:4">
@@ -7624,7 +7621,7 @@
         <v>82</v>
       </c>
       <c r="D28" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="29" spans="2:4">
@@ -7635,7 +7632,7 @@
         <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -7646,7 +7643,7 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="31" spans="2:4">
@@ -7657,7 +7654,7 @@
         <v>90</v>
       </c>
       <c r="D31" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="32" spans="2:4">
@@ -7668,7 +7665,7 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -7679,7 +7676,7 @@
         <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -7690,7 +7687,7 @@
         <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -7701,7 +7698,7 @@
         <v>102</v>
       </c>
       <c r="D35" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="36" spans="2:4">
@@ -7712,7 +7709,7 @@
         <v>105</v>
       </c>
       <c r="D36" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="37" spans="2:4">
@@ -7723,7 +7720,7 @@
         <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="38" spans="2:4">
@@ -7734,7 +7731,7 @@
         <v>111</v>
       </c>
       <c r="D38" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="39" spans="2:4">
@@ -7745,7 +7742,7 @@
         <v>114</v>
       </c>
       <c r="D39" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="40" spans="2:4">
@@ -7756,7 +7753,7 @@
         <v>117</v>
       </c>
       <c r="D40" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="41" spans="2:4">
@@ -7767,7 +7764,7 @@
         <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="42" spans="2:4">
@@ -7778,7 +7775,7 @@
         <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="43" spans="2:4">
@@ -7789,7 +7786,7 @@
         <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="44" spans="2:4">
@@ -7800,7 +7797,7 @@
         <v>129</v>
       </c>
       <c r="D44" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="45" spans="2:4">
@@ -7811,7 +7808,7 @@
         <v>132</v>
       </c>
       <c r="D45" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="46" spans="2:4">
@@ -7822,7 +7819,7 @@
         <v>135</v>
       </c>
       <c r="D46" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="47" spans="2:4">
@@ -7833,7 +7830,7 @@
         <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="48" spans="2:4">
@@ -7844,7 +7841,7 @@
         <v>141</v>
       </c>
       <c r="D48" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="49" spans="2:4">
@@ -7855,7 +7852,7 @@
         <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="50" spans="2:4">
@@ -7866,7 +7863,7 @@
         <v>147</v>
       </c>
       <c r="D50" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="51" spans="2:4">
@@ -7877,7 +7874,7 @@
         <v>150</v>
       </c>
       <c r="D51" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="52" spans="2:4">
@@ -7888,7 +7885,7 @@
         <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="53" spans="2:4">
@@ -7910,7 +7907,7 @@
         <v>159</v>
       </c>
       <c r="D54" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="55" spans="2:4">
@@ -7921,7 +7918,7 @@
         <v>162</v>
       </c>
       <c r="D55" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="56" spans="2:4">
@@ -7943,7 +7940,7 @@
         <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="58" spans="2:4">
@@ -7954,7 +7951,7 @@
         <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="59" spans="2:4">
@@ -7965,7 +7962,7 @@
         <v>174</v>
       </c>
       <c r="D59" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="60" spans="2:4">
@@ -7976,7 +7973,7 @@
         <v>132</v>
       </c>
       <c r="D60" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="61" spans="2:4">
@@ -7987,7 +7984,7 @@
         <v>178</v>
       </c>
       <c r="D61" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="62" spans="2:4">
@@ -7998,7 +7995,7 @@
         <v>181</v>
       </c>
       <c r="D62" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="63" spans="2:4">
@@ -8009,7 +8006,7 @@
         <v>184</v>
       </c>
       <c r="D63" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="64" spans="2:4">
@@ -8020,7 +8017,7 @@
         <v>187</v>
       </c>
       <c r="D64" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="65" spans="2:4">
@@ -8031,7 +8028,7 @@
         <v>190</v>
       </c>
       <c r="D65" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="66" spans="2:4">
@@ -8042,7 +8039,7 @@
         <v>192</v>
       </c>
       <c r="D66" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" spans="2:4">
@@ -8053,7 +8050,7 @@
         <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="68" spans="2:4">
@@ -8064,7 +8061,7 @@
         <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="69" spans="2:4">
@@ -8075,7 +8072,7 @@
         <v>201</v>
       </c>
       <c r="D69" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="70" spans="2:4">
@@ -8086,7 +8083,7 @@
         <v>204</v>
       </c>
       <c r="D70" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="71" spans="2:4">
@@ -8097,7 +8094,7 @@
         <v>207</v>
       </c>
       <c r="D71" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="72" spans="2:4">
@@ -8108,7 +8105,7 @@
         <v>210</v>
       </c>
       <c r="D72" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="73" spans="2:4">
@@ -8119,7 +8116,7 @@
         <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="74" spans="2:4">
@@ -8130,7 +8127,7 @@
         <v>216</v>
       </c>
       <c r="D74" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="75" spans="2:4">
@@ -8141,7 +8138,7 @@
         <v>219</v>
       </c>
       <c r="D75" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="76" spans="2:4">
@@ -8152,7 +8149,7 @@
         <v>222</v>
       </c>
       <c r="D76" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="77" spans="2:4">
@@ -8163,7 +8160,7 @@
         <v>225</v>
       </c>
       <c r="D77" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="78" spans="2:4">
@@ -8174,7 +8171,7 @@
         <v>228</v>
       </c>
       <c r="D78" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="79" spans="2:4">
@@ -8185,7 +8182,7 @@
         <v>231</v>
       </c>
       <c r="D79" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="80" spans="2:4">
@@ -8196,7 +8193,7 @@
         <v>234</v>
       </c>
       <c r="D80" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="81" spans="2:4">
@@ -8207,7 +8204,7 @@
         <v>237</v>
       </c>
       <c r="D81" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="82" spans="2:4">
@@ -8218,7 +8215,7 @@
         <v>240</v>
       </c>
       <c r="D82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="83" spans="2:4">
@@ -8240,7 +8237,7 @@
         <v>246</v>
       </c>
       <c r="D84" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="85" spans="2:4">
@@ -8251,7 +8248,7 @@
         <v>249</v>
       </c>
       <c r="D85" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="86" spans="2:4">
@@ -8262,7 +8259,7 @@
         <v>252</v>
       </c>
       <c r="D86" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="87" spans="2:4">
@@ -8273,7 +8270,7 @@
         <v>255</v>
       </c>
       <c r="D87" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="88" spans="2:4">
@@ -8284,7 +8281,7 @@
         <v>258</v>
       </c>
       <c r="D88" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="89" spans="2:4">
@@ -8295,7 +8292,7 @@
         <v>261</v>
       </c>
       <c r="D89" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="90" spans="2:4">
@@ -8306,7 +8303,7 @@
         <v>264</v>
       </c>
       <c r="D90" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="91" spans="2:4">
@@ -8317,7 +8314,7 @@
         <v>267</v>
       </c>
       <c r="D91" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="92" spans="2:4">
@@ -8328,7 +8325,7 @@
         <v>270</v>
       </c>
       <c r="D92" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="93" spans="2:4">
@@ -8339,7 +8336,7 @@
         <v>273</v>
       </c>
       <c r="D93" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="94" spans="2:4">
@@ -8350,7 +8347,7 @@
         <v>276</v>
       </c>
       <c r="D94" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="95" spans="2:4">
@@ -8361,7 +8358,7 @@
         <v>279</v>
       </c>
       <c r="D95" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="96" spans="2:4">
@@ -8372,7 +8369,7 @@
         <v>282</v>
       </c>
       <c r="D96" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="97" spans="2:4">
@@ -8383,7 +8380,7 @@
         <v>61</v>
       </c>
       <c r="D97" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="98" spans="2:4">

</xml_diff>

<commit_message>
fix in french app text: saison->disponibilite
</commit_message>
<xml_diff>
--- a/assets/i18n_data/app_text.xlsx
+++ b/assets/i18n_data/app_text.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22665" windowHeight="12795" activeTab="2"/>
+    <workbookView windowWidth="22665" windowHeight="12795" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="de" sheetId="1" r:id="rId1"/>
@@ -1546,7 +1546,7 @@
     <t>Informations légales</t>
   </si>
   <si>
-    <t>Données Saisonnières</t>
+    <t>Données de disponibilité</t>
   </si>
   <si>
     <t>Protection des données</t>
@@ -1623,7 +1623,7 @@
     <t>Septembre</t>
   </si>
   <si>
-    <t>Filtrer par saison</t>
+    <t>Filtrer par disponibilité</t>
   </si>
   <si>
     <t>L'application redémarre lorsque la langue est changée</t>
@@ -1650,7 +1650,7 @@
     <t>Par défaut : Europe centrale</t>
   </si>
   <si>
-    <t>Trier par saison</t>
+    <t>Trier par disponibilité</t>
   </si>
   <si>
     <t>p. ex. coings, mûres des marais</t>
@@ -1958,10 +1958,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1987,26 +1987,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2018,16 +2003,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2042,10 +2019,17 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2058,14 +2042,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2079,24 +2087,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2115,6 +2107,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -2125,13 +2125,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2143,49 +2263,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2197,61 +2275,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2263,49 +2305,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2328,6 +2328,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -2339,11 +2378,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2363,51 +2408,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -2419,118 +2419,118 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2539,22 +2539,22 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -5108,7 +5108,7 @@
   <sheetPr/>
   <dimension ref="B1:D98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A63" workbookViewId="0">
       <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
@@ -6207,8 +6207,8 @@
   <sheetPr/>
   <dimension ref="B1:D98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>

</xml_diff>

<commit_message>
added italian and bulgarian translations from local shelf to repo
</commit_message>
<xml_diff>
--- a/assets/i18n_data/app_text.xlsx
+++ b/assets/i18n_data/app_text.xlsx
@@ -12,13 +12,15 @@
     <sheet name="es" sheetId="3" r:id="rId3"/>
     <sheet name="fr" sheetId="4" r:id="rId4"/>
     <sheet name="pl" sheetId="5" r:id="rId5"/>
+    <sheet name="it" sheetId="6" r:id="rId6"/>
+    <sheet name="bg" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2058" uniqueCount="821">
   <si>
     <t>key</t>
   </si>
@@ -1951,6 +1953,553 @@
   </si>
   <si>
     <t>Wsparcie</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>I prodotti freschi sono più genuini e salutari per il tuo corpo.</t>
+  </si>
+  <si>
+    <t>I cibi freschi sono generalmente più economici.</t>
+  </si>
+  <si>
+    <t>I costi per la conservazione dei cibi si riducono.</t>
+  </si>
+  <si>
+    <t>I trasporti sono meno pericolosi per l'ambiente.</t>
+  </si>
+  <si>
+    <t>Supporti il commercio locale.</t>
+  </si>
+  <si>
+    <t>Nota bene che la reale disponibilità di cibi nella tua zona può differire dalle informazioni mostrate.</t>
+  </si>
+  <si>
+    <t>Perché preoccuparsi della stagionalità dei cibi?</t>
+  </si>
+  <si>
+    <t>Da quando tutti i cibi sono disponibili durante l'intero arco dell'anno, le persone hanno cominciato a dimenticarsi dell'importanza dei cibi di stagione, nonostante comprare cibi locali e di stagione porti spesso a significativi vantaggi:</t>
+  </si>
+  <si>
+    <t>Informazioni sull'app</t>
+  </si>
+  <si>
+    <t>Questa app ti consente di mangiare meglio spendendo meno, migliorando anche la consapevolezza sull'origine dei cibi.</t>
+  </si>
+  <si>
+    <t>Calendario dei cibi di stagione</t>
+  </si>
+  <si>
+    <t>Aprile</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Indietro</t>
+  </si>
+  <si>
+    <t>Europa centrale</t>
+  </si>
+  <si>
+    <t>Il codice sorgente di questa app è disponibile su GitHub:</t>
+  </si>
+  <si>
+    <t>Vai alla repository GitHub</t>
+  </si>
+  <si>
+    <t>Mostrami il codice!</t>
+  </si>
+  <si>
+    <t>Se hai trovato un errore o hai suggerimenti, contattami attraverso il mio sito Web.</t>
+  </si>
+  <si>
+    <t>Vai al sito Web</t>
+  </si>
+  <si>
+    <t>Manca qualcosa o hai trovato un errore?</t>
+  </si>
+  <si>
+    <t>Contribuisci</t>
+  </si>
+  <si>
+    <t>Dicembre</t>
+  </si>
+  <si>
+    <t>Controlla le impostazioni del filtro per i cibi.</t>
+  </si>
+  <si>
+    <t>Aggiungi un cibo ai preferiti toccando la stella ☆.</t>
+  </si>
+  <si>
+    <t>Nessun preferito presente!</t>
+  </si>
+  <si>
+    <t>Nessun cibo disponibile!</t>
+  </si>
+  <si>
+    <t>Nessun cibo trovato!</t>
+  </si>
+  <si>
+    <t>Febbraio</t>
+  </si>
+  <si>
+    <t>Importato da molto lontano, principalmente tramite trasporto aereo.</t>
+  </si>
+  <si>
+    <t>Importanto da lontano, principalmente tramite trasporto terrestre.</t>
+  </si>
+  <si>
+    <t>Di stagione o disponibile localmente/regionalmente.</t>
+  </si>
+  <si>
+    <t>Importato da molto lontano, principalmente tramite trasporto navale.</t>
+  </si>
+  <si>
+    <t>Il colore dello sfondo del nome corrisponde alla suddetta classificatione. Verde è migliore di rosso.</t>
+  </si>
+  <si>
+    <t>Questa app mostra velocemente quali sono i cibi di stagione al momento:</t>
+  </si>
+  <si>
+    <t>Come utilizzare l'app?</t>
+  </si>
+  <si>
+    <t>Toccando la stella ☆ di un cibo, lo aggiungi o rimuovi dalla tua lista di preferiti. Toccando la stella nella barra del menù, puoi visualizzare i tuoi preferiti.</t>
+  </si>
+  <si>
+    <t>Un'icona nera indica elevata disponibilità, un'icona grigia indica limitata disponibilità.</t>
+  </si>
+  <si>
+    <t>Istruzioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licenza: </t>
+  </si>
+  <si>
+    <t>Creatore:</t>
+  </si>
+  <si>
+    <t>Informazioni legali</t>
+  </si>
+  <si>
+    <t>Dati sulla disponibilità dei cibi</t>
+  </si>
+  <si>
+    <t>Informativa sulla privacy</t>
+  </si>
+  <si>
+    <t>Utilizzando questa app, nessun dato personale viene raccolto o trattato. Per modificare e salvare le impostazioni, è richiesto il permesso di accesso alla memoria del dispositivo.</t>
+  </si>
+  <si>
+    <t>Lebensmittellexikon.de (la maggior parte);
+Andreas Boltres (il resto).</t>
+  </si>
+  <si>
+    <t>Un ringranziamento particolare al team di Lebensmittellexikon.de per aver permesso l'utilizzo dei dati sulla disponibilità dei cibi!</t>
+  </si>
+  <si>
+    <t>Il contenuto di questa app è stato creato con la massima cura e in buona fede, tuttavia è reso disponibile senza alcuna garanzia, esplicita o implicita, riguardo all'accuratezza, la validità, l'affidabilità o la completezza delle informazioni ivi mostrate.</t>
+  </si>
+  <si>
+    <t>Font Awesome 5 (logo mela, logo carota)
+(Licenza: fontawesome.com/license)</t>
+  </si>
+  <si>
+    <t>Immagini</t>
+  </si>
+  <si>
+    <t>Editore</t>
+  </si>
+  <si>
+    <t>Fonti</t>
+  </si>
+  <si>
+    <t>Testo dell'app</t>
+  </si>
+  <si>
+    <t>Traduzioni</t>
+  </si>
+  <si>
+    <t>Gennaio</t>
+  </si>
+  <si>
+    <t>Luglio</t>
+  </si>
+  <si>
+    <t>Giugno</t>
+  </si>
+  <si>
+    <t>Italiano</t>
+  </si>
+  <si>
+    <t>Maggio</t>
+  </si>
+  <si>
+    <t>Tutti i cibi disponibili</t>
+  </si>
+  <si>
+    <t>Nessun cibo importato oltreoceano/da molto lontano</t>
+  </si>
+  <si>
+    <t>Solo cibi regionali/locali</t>
+  </si>
+  <si>
+    <t>Nessun cibo importato tramite trasporto aereo</t>
+  </si>
+  <si>
+    <t>Ottobre</t>
+  </si>
+  <si>
+    <t>Cerca...</t>
+  </si>
+  <si>
+    <t>Settembre</t>
+  </si>
+  <si>
+    <t>Filtra in base alla disponibilità</t>
+  </si>
+  <si>
+    <t>Cambiare la lingua riavvierà l'app</t>
+  </si>
+  <si>
+    <t>Lingua</t>
+  </si>
+  <si>
+    <t>Utilizza la lingua di sistema</t>
+  </si>
+  <si>
+    <t>Utilizza l'inglese se la lingua di sistema non è supportata</t>
+  </si>
+  <si>
+    <t>Impostazioni</t>
+  </si>
+  <si>
+    <t>Regione</t>
+  </si>
+  <si>
+    <t>Utilizza la regione di sistema</t>
+  </si>
+  <si>
+    <t>Utilizza 'Europa centrale' se la regione di sistema non è supportata</t>
+  </si>
+  <si>
+    <t>Ordina per disponibilità</t>
+  </si>
+  <si>
+    <t>es. mela cotogna, camemoro</t>
+  </si>
+  <si>
+    <t>Mostra cibi speciali e insoliti</t>
+  </si>
+  <si>
+    <t>Versione</t>
+  </si>
+  <si>
+    <t>Dona</t>
+  </si>
+  <si>
+    <t>Ne sono davvero felice! Il mosto migliore per supportarmi è fare passaparola: fai conoscere alla tua famiglia e ai tuoi amici questa app!</t>
+  </si>
+  <si>
+    <t>In questo modo possiamo incrementare la consapevolezza sulle origini dei cibi e al contempo risparmiare e mangiare meglio.</t>
+  </si>
+  <si>
+    <t>Ti piace l'app?</t>
+  </si>
+  <si>
+    <t>Quest'app rimarrà completamente gratuita e priva di pubblicità fino a quando sarà in sviluppo.</t>
+  </si>
+  <si>
+    <t>Ma se ti andasse di aiutare, potresti dare un'occhiata a cosa faccio in generale nel mio sito Web.</t>
+  </si>
+  <si>
+    <t>Supporta</t>
+  </si>
+  <si>
+    <t>bg</t>
+  </si>
+  <si>
+    <t>Пресните продукти имат по-добър вкус и са по-здравословни за вашето тяло.</t>
+  </si>
+  <si>
+    <t>Пресните храни обикновено са по-евтини.</t>
+  </si>
+  <si>
+    <t>Усилията, положени за съхранение на храни, са намалени.</t>
+  </si>
+  <si>
+    <t>Транспортът е по-малко вреден за околната среда.</t>
+  </si>
+  <si>
+    <t>Вие подкрепяте местния бизнес и работни места.</t>
+  </si>
+  <si>
+    <t>Моля, имайте предвид, че действителната наличност на храни в местния супермаркет може да се различава от информацията, показана тук.</t>
+  </si>
+  <si>
+    <t>Защо да ни е грижа за сезоните на храните?</t>
+  </si>
+  <si>
+    <t>В днешно време, тъй като почти всички храни са достъпни през цялата година, хората не нямат представа за сезонността на своите храни. Купуването на сезонни и местни храни обаче често има поразителни предимства:</t>
+  </si>
+  <si>
+    <t>Относно приложението</t>
+  </si>
+  <si>
+    <t>Това приложение ви позволява да се храните по-евтино и по-вкусно и повишава информираността за произхода на нашата храна.</t>
+  </si>
+  <si>
+    <t>Календар на сезонните храни</t>
+  </si>
+  <si>
+    <t>Април</t>
+  </si>
+  <si>
+    <t>Август</t>
+  </si>
+  <si>
+    <t>Назад</t>
+  </si>
+  <si>
+    <t>Централна Европа</t>
+  </si>
+  <si>
+    <t>Изходният код за приложението е достъпен на GitHub:</t>
+  </si>
+  <si>
+    <t>Към репото на GitHub</t>
+  </si>
+  <si>
+    <t>Покажете ми кода!</t>
+  </si>
+  <si>
+    <t>Ако сте открили грешка или място за конкретно подобрение, не се колебайте да се свържете с мен чрез моята уеб страница.</t>
+  </si>
+  <si>
+    <t>Към уеб страницата</t>
+  </si>
+  <si>
+    <t>Нещо липсва или не е наред?</t>
+  </si>
+  <si>
+    <t>Допринесете</t>
+  </si>
+  <si>
+    <t>Декември</t>
+  </si>
+  <si>
+    <t>Проверете филтрите за вашите храни.</t>
+  </si>
+  <si>
+    <t>Добавете фаворит, като докоснете звездата на храната ☆.</t>
+  </si>
+  <si>
+    <t>Няма налични фаворити!</t>
+  </si>
+  <si>
+    <t>Няма налични храни!</t>
+  </si>
+  <si>
+    <t>Не са намерени храни!</t>
+  </si>
+  <si>
+    <t>Февруари</t>
+  </si>
+  <si>
+    <t>Внос от далеч, най-вече със самолет.</t>
+  </si>
+  <si>
+    <t>Внос от не много далеч, най-вече чрез сухопътен транспорт.</t>
+  </si>
+  <si>
+    <t>Е сезонен/на разположение на местно или регионално ниво.</t>
+  </si>
+  <si>
+    <t>Внос от далеч, предимно по кораб.</t>
+  </si>
+  <si>
+    <t>Цветът на полето за име показва, че съответства на горната класификация. Зелено е по-добро от червено.</t>
+  </si>
+  <si>
+    <t>Това приложение ви показва с един поглед кои храни са в сезон в момента:</t>
+  </si>
+  <si>
+    <t>Как да използвам приложението?</t>
+  </si>
+  <si>
+    <t>Докосвайки звездата на храната ☆, вие я добавяте към/премахвате от списъка си с любими. Докосването на звездата в лентата с менюта ви позволява да ограничите изгледа до вашите любими.</t>
+  </si>
+  <si>
+    <t>Черна икона показва изобилие от наличност, сива икона ограничена наличност от тази конкретна категория.</t>
+  </si>
+  <si>
+    <t>Обяснение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лиценз: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Създател: </t>
+  </si>
+  <si>
+    <t>Информация за приложението</t>
+  </si>
+  <si>
+    <t>Отпечатък</t>
+  </si>
+  <si>
+    <t>Данни за наличност</t>
+  </si>
+  <si>
+    <t>Политика за поверителност</t>
+  </si>
+  <si>
+    <t>Използвайки това приложение не се събират лични данни. За да запазите и заредите настройките на приложението, е необходимо разрешение за достъп до хранилището на устройството.</t>
+  </si>
+  <si>
+    <t>Lebensmittellexikon.de (основни части);
+Андреас Болтрес (останалите).</t>
+  </si>
+  <si>
+    <t>Благодарности на екипа на Lebensmittellexikon.de, благодаря, че ми позволихте да използвам вашите данни за наличност!</t>
+  </si>
+  <si>
+    <t>Опровержение</t>
+  </si>
+  <si>
+    <t>Съдържанието на това приложение е създадено и се предоставя добросъвестно с изключително внимание. Въпреки това не давам никакви изявления или гаранции от какъвто и да е вид, изрични или подразбиращи се, относно точността, адекватността, валидността, надеждността, наличността или пълнотата на каквато и да е информация, показана в това приложение.</t>
+  </si>
+  <si>
+    <t>Шрифт</t>
+  </si>
+  <si>
+    <t>Шрифт Awesome 5 (лого на ябълка, лого на моркови)
+(Лиценз: fontawesome.com/license)</t>
+  </si>
+  <si>
+    <t>Изображения</t>
+  </si>
+  <si>
+    <t>Андреас Болтрес</t>
+  </si>
+  <si>
+    <t>Издател</t>
+  </si>
+  <si>
+    <t>Източници</t>
+  </si>
+  <si>
+    <t>Текст на приложението</t>
+  </si>
+  <si>
+    <t>Преводи</t>
+  </si>
+  <si>
+    <t>Януари</t>
+  </si>
+  <si>
+    <t>Юли</t>
+  </si>
+  <si>
+    <t>Юни</t>
+  </si>
+  <si>
+    <t>Български</t>
+  </si>
+  <si>
+    <t>Март</t>
+  </si>
+  <si>
+    <t>Май</t>
+  </si>
+  <si>
+    <t>Всички налични храни</t>
+  </si>
+  <si>
+    <t>Няма храни, внесени от чужбина/далеч</t>
+  </si>
+  <si>
+    <t>Само местни и регионални храни</t>
+  </si>
+  <si>
+    <t>Няма храни, внесени със самолет</t>
+  </si>
+  <si>
+    <t>Ноември</t>
+  </si>
+  <si>
+    <t>Октомври</t>
+  </si>
+  <si>
+    <t>Търсене...</t>
+  </si>
+  <si>
+    <t>Септември</t>
+  </si>
+  <si>
+    <t>Филтрирайте по наличност</t>
+  </si>
+  <si>
+    <t>Промяната на езика рестартира приложението</t>
+  </si>
+  <si>
+    <t>Език</t>
+  </si>
+  <si>
+    <t>Използвайте езика на устройството</t>
+  </si>
+  <si>
+    <t>Използва английски, ако езикът на устройството не се поддържа</t>
+  </si>
+  <si>
+    <t>Настройки</t>
+  </si>
+  <si>
+    <t>Регион</t>
+  </si>
+  <si>
+    <t>Използвайте региона на устройството</t>
+  </si>
+  <si>
+    <t>Използва „Централна Европа“, ако регионът на устройството не се поддържа</t>
+  </si>
+  <si>
+    <t>Сортирай по наличност</t>
+  </si>
+  <si>
+    <t>напр. дюля, боровинка</t>
+  </si>
+  <si>
+    <t>Покажете специални и необичайни храни</t>
+  </si>
+  <si>
+    <t>Версия</t>
+  </si>
+  <si>
+    <t>Дайте милостиня</t>
+  </si>
+  <si>
+    <t>Хубаво е да чуеш, че! Най-ефективният начин да ме подкрепите е просто да споделите проекта: Нека вашите приятели и семейство знаят за приложението!</t>
+  </si>
+  <si>
+    <t>По този начин можем да повишим осведомеността за произхода на нашите храни заедно, като същевременно спестяваме пари и се храним по-вкусно.</t>
+  </si>
+  <si>
+    <t>Харесвате ли приложението?</t>
+  </si>
+  <si>
+    <t>Това приложение ще остане напълно безплатно и без реклами, докато го разработвам аз.</t>
+  </si>
+  <si>
+    <t>Но ако искате да подкрепите работата ми, можете да погледнете какво правя по принцип на уеб страницата ми.</t>
+  </si>
+  <si>
+    <t>Поддържа</t>
+  </si>
+  <si>
+    <t>Уикипедия</t>
   </si>
 </sst>
 </file>
@@ -1958,18 +2507,38 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="0"/>
     </font>
     <font>
       <u/>
@@ -1981,7 +2550,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1995,8 +2586,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2012,30 +2627,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2049,33 +2641,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2095,22 +2679,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2125,37 +2694,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2167,49 +2718,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2227,13 +2736,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2245,67 +2868,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2319,11 +2888,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2345,50 +2953,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2417,207 +2986,219 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+  </cellStyleXfs>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="50">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
+    <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="4" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="5" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="6" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="7" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="9" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="10" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="11" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="14" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="15" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="16" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="17" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="18" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="21" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="22" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="23" builtinId="32"/>
+    <cellStyle name="Bad" xfId="24" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="25" builtinId="42"/>
+    <cellStyle name="Total" xfId="26" builtinId="25"/>
+    <cellStyle name="Output" xfId="27" builtinId="21"/>
+    <cellStyle name="Currency" xfId="28" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="29" builtinId="38"/>
+    <cellStyle name="Note" xfId="30" builtinId="10"/>
+    <cellStyle name="Input" xfId="31" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="32" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="33" builtinId="22"/>
+    <cellStyle name="Good" xfId="34" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="35" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="36" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="37" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="38" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50"/>
+    <cellStyle name="Title" xfId="40" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="41" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="42" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -5466,7 +6047,7 @@
       <c r="C32" t="s">
         <v>93</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="7" t="s">
         <v>404</v>
       </c>
     </row>
@@ -5477,7 +6058,7 @@
       <c r="C33" t="s">
         <v>96</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="7" t="s">
         <v>405</v>
       </c>
     </row>
@@ -5488,7 +6069,7 @@
       <c r="C34" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="7" t="s">
         <v>406</v>
       </c>
     </row>
@@ -5499,7 +6080,7 @@
       <c r="C35" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="7" t="s">
         <v>407</v>
       </c>
     </row>
@@ -5510,7 +6091,7 @@
       <c r="C36" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="7" t="s">
         <v>408</v>
       </c>
     </row>
@@ -5521,7 +6102,7 @@
       <c r="C37" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="7" t="s">
         <v>409</v>
       </c>
     </row>
@@ -5532,7 +6113,7 @@
       <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="7" t="s">
         <v>410</v>
       </c>
     </row>
@@ -5543,7 +6124,7 @@
       <c r="C39" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="7" t="s">
         <v>411</v>
       </c>
     </row>
@@ -5565,7 +6146,7 @@
       <c r="C41" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="7" t="s">
         <v>413</v>
       </c>
     </row>
@@ -8398,4 +8979,2211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:D98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="7.925" style="4"/>
+    <col min="2" max="2" width="28.025" style="4"/>
+    <col min="3" max="3" width="18.475" style="4"/>
+    <col min="4" max="4" width="20.7083333333333" style="4"/>
+    <col min="5" max="16384" width="7.925" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="49" ht="54" spans="2:4">
+      <c r="B49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" ht="67.5" spans="2:4">
+      <c r="B54" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter alignWithMargins="0" scaleWithDoc="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:D98"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="30.9" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83.2833333333333" style="1" customWidth="1"/>
+    <col min="4" max="4" width="244.55" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
+      <c r="B24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
+      <c r="B25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
+      <c r="B26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
+      <c r="B27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4">
+      <c r="B29" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4">
+      <c r="B30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4">
+      <c r="B31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4">
+      <c r="B32" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
+      <c r="B33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
+      <c r="B34" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
+      <c r="B35" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
+      <c r="B36" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
+      <c r="B37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
+      <c r="B38" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
+      <c r="B39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
+      <c r="B40" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
+      <c r="B41" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
+      <c r="B42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
+      <c r="B44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
+      <c r="B45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
+      <c r="B46" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
+      <c r="B47" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
+      <c r="B48" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="49" ht="27" spans="2:4">
+      <c r="B49" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4">
+      <c r="B50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4">
+      <c r="B51" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4">
+      <c r="B52" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4">
+      <c r="B53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="54" ht="27" spans="2:4">
+      <c r="B54" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4">
+      <c r="B55" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4">
+      <c r="B56" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4">
+      <c r="B57" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4">
+      <c r="B58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4">
+      <c r="B59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4">
+      <c r="B60" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4">
+      <c r="B61" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4">
+      <c r="B62" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4">
+      <c r="B63" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4">
+      <c r="B64" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4">
+      <c r="B65" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4">
+      <c r="B66" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4">
+      <c r="B67" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4">
+      <c r="B68" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4">
+      <c r="B69" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4">
+      <c r="B70" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4">
+      <c r="B71" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4">
+      <c r="B72" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4">
+      <c r="B73" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4">
+      <c r="B74" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4">
+      <c r="B75" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4">
+      <c r="B76" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4">
+      <c r="B77" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4">
+      <c r="B78" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4">
+      <c r="B79" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4">
+      <c r="B80" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4">
+      <c r="B82" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4">
+      <c r="B83" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4">
+      <c r="B85" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4">
+      <c r="B86" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4">
+      <c r="B87" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4">
+      <c r="B88" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4">
+      <c r="B89" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4">
+      <c r="B90" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4">
+      <c r="B91" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4">
+      <c r="B92" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4">
+      <c r="B93" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4">
+      <c r="B94" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4">
+      <c r="B95" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4">
+      <c r="B96" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4">
+      <c r="B97" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4">
+      <c r="B98" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>820</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>